<commit_message>
Cleaned up and refreshed matches. Verified scores of playoff games. Included final stats.
</commit_message>
<xml_diff>
--- a/combined_stats.xlsx
+++ b/combined_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab4ea91dc20bd738/Documents/GitHub/DUOACHCATT-5-15-21-STATS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_99BB30C2AF14D40860B1A384D8AB76E111354059" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_B7F733D1D964D102773F0966314B6BE111356257" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1ABED312-D0AF-4FAE-80E0-E544C76651CF}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team Stats" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>win</t>
   </si>
@@ -102,49 +102,46 @@
     <t>Will Reuter</t>
   </si>
   <si>
+    <t>Abigail Friedstrom</t>
+  </si>
+  <si>
     <t>Scott Youngquist</t>
   </si>
   <si>
-    <t>Abigail Friedstrom</t>
-  </si>
-  <si>
     <t>La Maestra (Parker Johnson)</t>
   </si>
   <si>
+    <t>Ky Reckamp</t>
+  </si>
+  <si>
+    <t>Patty (Patrick Wells)</t>
+  </si>
+  <si>
     <t>Noah Mcredmond</t>
   </si>
   <si>
-    <t>Ky Reckamp</t>
-  </si>
-  <si>
     <t>Clete Reinberger</t>
   </si>
   <si>
+    <t>Aidan Hook</t>
+  </si>
+  <si>
+    <t>GHAS (Andrew Ghastine)</t>
+  </si>
+  <si>
+    <t>El Rey de Rompecabezas (Mr. Cool)</t>
+  </si>
+  <si>
+    <t>Axe (Hildy)</t>
+  </si>
+  <si>
     <t>Sir Wheeze (Marcus Daley)</t>
   </si>
   <si>
-    <t>Aidan Hook</t>
-  </si>
-  <si>
     <t>Duke Hogs (Hogan Daley)</t>
   </si>
   <si>
-    <t>Patty (Patrick Wells)</t>
-  </si>
-  <si>
-    <t>GHAS (Andrew Ghastine)</t>
-  </si>
-  <si>
-    <t>Axe (Hildy)</t>
-  </si>
-  <si>
     <t>Faith Youngquist</t>
-  </si>
-  <si>
-    <t>El Rey de Rompecabezas (Mr. Cool)</t>
-  </si>
-  <si>
-    <t>#NAME?</t>
   </si>
 </sst>
 </file>
@@ -548,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -609,7 +606,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -621,40 +618,40 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>73.5</v>
+        <v>75.333333333333329</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
       <c r="H2">
-        <v>7.25</v>
+        <v>18.333333333333329</v>
       </c>
       <c r="I2">
-        <v>30.25</v>
+        <v>28.666666666666671</v>
       </c>
       <c r="J2">
-        <v>15.25</v>
+        <v>17.166666666666671</v>
       </c>
       <c r="K2">
-        <v>28</v>
+        <v>29.5</v>
       </c>
       <c r="L2">
-        <v>294</v>
+        <v>452</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="N2">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="O2">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="P2">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="Q2">
-        <v>112</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.45">
@@ -662,52 +659,52 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F3">
-        <v>53.75</v>
+        <v>51.5</v>
       </c>
       <c r="G3">
-        <v>2.75</v>
+        <v>2.833333333333333</v>
       </c>
       <c r="H3">
-        <v>7.75</v>
+        <v>10</v>
       </c>
       <c r="I3">
-        <v>22</v>
+        <v>20.666666666666671</v>
       </c>
       <c r="J3">
-        <v>11.75</v>
+        <v>11.83333333333333</v>
       </c>
       <c r="K3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3">
-        <v>215</v>
+        <v>309</v>
       </c>
       <c r="M3">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="N3">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="O3">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="P3">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="Q3">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.45">
@@ -715,113 +712,113 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F4">
-        <v>50.25</v>
+        <v>50.333333333333343</v>
       </c>
       <c r="G4">
-        <v>1.25</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="H4">
-        <v>5.5</v>
+        <v>11.66666666666667</v>
       </c>
       <c r="I4">
         <v>16.5</v>
       </c>
       <c r="J4">
-        <v>9.5</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="K4">
-        <v>24.25</v>
+        <v>23.166666666666671</v>
       </c>
       <c r="L4">
-        <v>201</v>
+        <v>302</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="N4">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="O4">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="P4">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="Q4">
-        <v>97</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F5">
-        <v>47</v>
+        <v>51.166666666666657</v>
       </c>
       <c r="G5">
-        <v>0.25</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="H5">
-        <v>5.25</v>
+        <v>10.16666666666667</v>
       </c>
       <c r="I5">
-        <v>13.25</v>
+        <v>15.66666666666667</v>
       </c>
       <c r="J5">
-        <v>12.25</v>
+        <v>13</v>
       </c>
       <c r="K5">
-        <v>21.5</v>
+        <v>22.5</v>
       </c>
       <c r="L5">
-        <v>188</v>
+        <v>307</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="N5">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="O5">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="P5">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="Q5">
-        <v>86</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -830,43 +827,43 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F6">
-        <v>49.25</v>
+        <v>51.333333333333343</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>13.66666666666667</v>
       </c>
       <c r="I6">
-        <v>15.25</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>13.75</v>
+        <v>12.83333333333333</v>
       </c>
       <c r="K6">
-        <v>20.25</v>
+        <v>23.5</v>
       </c>
       <c r="L6">
-        <v>197</v>
+        <v>308</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="N6">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="O6">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="P6">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Q6">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
@@ -874,63 +871,63 @@
         <v>21</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F7">
-        <v>44.5</v>
+        <v>45.5</v>
       </c>
       <c r="G7">
-        <v>1.75</v>
+        <v>2</v>
       </c>
       <c r="H7">
-        <v>7.75</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="I7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J7">
-        <v>9.25</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="K7">
-        <v>21.25</v>
+        <v>21.333333333333329</v>
       </c>
       <c r="L7">
-        <v>178</v>
+        <v>273</v>
       </c>
       <c r="M7">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="N7">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="O7">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="P7">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="Q7">
-        <v>85</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -939,51 +936,51 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>24.5</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="G8">
-        <v>0.25</v>
+        <v>1.2</v>
       </c>
       <c r="H8">
-        <v>3.5</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="I8">
-        <v>10.25</v>
+        <v>9.6</v>
       </c>
       <c r="J8">
-        <v>6</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="K8">
-        <v>8.25</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="L8">
-        <v>98</v>
+        <v>184</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="N8">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="O8">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="P8">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="Q8">
-        <v>33</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -992,40 +989,40 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>35</v>
+        <v>21.8</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="H9">
-        <v>1.75</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I9">
-        <v>8.25</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="J9">
-        <v>9.5</v>
+        <v>5.6</v>
       </c>
       <c r="K9">
-        <v>17.25</v>
+        <v>7.4</v>
       </c>
       <c r="L9">
-        <v>140</v>
+        <v>109</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N9">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="O9">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="P9">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="Q9">
-        <v>69</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1035,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1071,25 +1068,25 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>29.5</v>
+        <v>28.833333333333329</v>
       </c>
       <c r="C2">
-        <v>2.5</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="D2">
+        <v>11.66666666666667</v>
+      </c>
+      <c r="E2">
         <v>11</v>
       </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
       <c r="F2">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="G2">
-        <v>59</v>
+        <v>173</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -1097,25 +1094,25 @@
         <v>26</v>
       </c>
       <c r="B3">
-        <v>26.666666666666671</v>
+        <v>28.666666666666671</v>
       </c>
       <c r="C3">
-        <v>3.333333333333333</v>
+        <v>2.333333333333333</v>
       </c>
       <c r="D3">
-        <v>8.3333333333333339</v>
+        <v>10.83333333333333</v>
       </c>
       <c r="E3">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="G3">
-        <v>80</v>
+        <v>172</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -1123,25 +1120,25 @@
         <v>27</v>
       </c>
       <c r="B4">
-        <v>18.5</v>
+        <v>23.5</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>2.5</v>
       </c>
       <c r="D4">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G4">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -1149,25 +1146,25 @@
         <v>28</v>
       </c>
       <c r="B5">
-        <v>18.5</v>
+        <v>21.833333333333329</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="D5">
-        <v>8.5</v>
+        <v>9.1666666666666661</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="G5">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -1175,25 +1172,25 @@
         <v>29</v>
       </c>
       <c r="B6">
-        <v>14.66666666666667</v>
+        <v>18.5</v>
       </c>
       <c r="C6">
-        <v>1.333333333333333</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="D6">
-        <v>5.333333333333333</v>
+        <v>7.5</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F6">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G6">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -1201,25 +1198,25 @@
         <v>30</v>
       </c>
       <c r="B7">
-        <v>13.5</v>
+        <v>18.5</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F7">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G7">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
@@ -1227,25 +1224,25 @@
         <v>31</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>16.666666666666671</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>6.833333333333333</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="G8">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="H8">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
@@ -1253,25 +1250,25 @@
         <v>32</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>13.66666666666667</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G9">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -1279,25 +1276,25 @@
         <v>33</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>13.6</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="D10">
+        <v>5.6</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
       <c r="F10">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
@@ -1305,25 +1302,25 @@
         <v>34</v>
       </c>
       <c r="B11">
-        <v>7.5</v>
+        <v>11.83333333333333</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>1.833333333333333</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>3.166666666666667</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F11">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="G11">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
@@ -1331,25 +1328,25 @@
         <v>35</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>11.5</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G12">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -1357,25 +1354,25 @@
         <v>36</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>10.4</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D13">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="F13">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -1383,25 +1380,25 @@
         <v>37</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G14">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -1409,25 +1406,25 @@
         <v>38</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>5.25</v>
       </c>
       <c r="C15">
-        <v>0.33333333333333331</v>
+        <v>0.25</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>2.25</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G15">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -1435,51 +1432,25 @@
         <v>39</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G16">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="H16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
@@ -1508,10 +1481,10 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -1519,7 +1492,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -1530,10 +1503,10 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1541,10 +1514,10 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1552,10 +1525,10 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -1563,10 +1536,10 @@
         <v>21</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1577,7 +1550,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>